<commit_message>
Updated the computation of the fields.
</commit_message>
<xml_diff>
--- a/b11_1/fields/fields_with_relations_and_constraints.xlsx
+++ b/b11_1/fields/fields_with_relations_and_constraints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yann/Prog/Python/LBA/b11_1/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6959CAB2-7FF3-884C-AC8A-ABD02E602B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCE1A61-DA3A-B643-8FF0-A0C1610A6B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20640" windowHeight="20620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Lieferant" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="109">
   <si>
     <t>Positions-Nr.</t>
   </si>
@@ -808,7 +808,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -856,6 +856,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1140,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1878,7 +1881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45268E68-3979-422D-9E08-1E63DD4A2AF3}">
   <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1990,7 +1993,9 @@
       <c r="D7" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="25" t="s">
+        <v>93</v>
+      </c>
       <c r="F7" s="22"/>
       <c r="G7" s="2" t="s">
         <v>100</v>
@@ -2210,7 +2215,7 @@
         <v>59</v>
       </c>
       <c r="D21" s="23"/>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="27" t="s">
         <v>93</v>
       </c>
       <c r="F21" s="24"/>

</xml_diff>